<commit_message>
modify list of deliverables
</commit_message>
<xml_diff>
--- a/08_Management/List_of_Deliverables-BCD1-0117_BCDCarpentryProject.xlsx
+++ b/08_Management/List_of_Deliverables-BCD1-0117_BCDCarpentryProject.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="22">
   <si>
     <t>Deliverable's Name</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -97,6 +97,10 @@
   </si>
   <si>
     <t>User Manual</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Progress Report</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -480,10 +484,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -673,9 +677,20 @@
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A18" s="2">
+        <v>17</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C18" s="2" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>